<commit_message>
solved new questions 17/01
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\study\python\Love Babbar 450 questions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\study\python\DS-450-python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5F2FA1F-9F45-4C6C-A5EB-81A222C49541}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59098A71-FEA4-46C1-A307-A98D41C7471E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7755" yWindow="2430" windowWidth="28800" windowHeight="11385" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="8100" yWindow="2775" windowWidth="28800" windowHeight="11385" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1855,7 +1855,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A344" workbookViewId="0">
-      <selection activeCell="C360" sqref="C360"/>
+      <selection activeCell="D353" sqref="D353"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -5599,7 +5599,7 @@
         <v>345</v>
       </c>
       <c r="C357" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="358" spans="1:3" ht="21">
@@ -5610,7 +5610,7 @@
         <v>346</v>
       </c>
       <c r="C358" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="359" spans="1:3" ht="21">
@@ -5632,7 +5632,7 @@
         <v>348</v>
       </c>
       <c r="C360" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="361" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Solved Some Linked List question 158, 159, 160, 161, 162
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\study\python\DS-450-python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30CEB793-337C-406A-9A93-C8D602C1FD4F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C303A9A2-C101-4775-A7AE-D44F1E567100}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1854,8 +1854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B167" workbookViewId="0">
-      <selection activeCell="C363" sqref="C363"/>
+    <sheetView tabSelected="1" topLeftCell="A149" workbookViewId="0">
+      <selection activeCell="C163" sqref="C163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3510,7 +3510,7 @@
         <v>154</v>
       </c>
       <c r="C158" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="159" spans="1:3" ht="21">
@@ -3521,7 +3521,7 @@
         <v>155</v>
       </c>
       <c r="C159" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="160" spans="1:3" ht="21">
@@ -3543,7 +3543,7 @@
         <v>157</v>
       </c>
       <c r="C161" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="162" spans="1:3" ht="21">
@@ -3554,7 +3554,7 @@
         <v>158</v>
       </c>
       <c r="C162" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="163" spans="1:3" ht="21">

</xml_diff>

<commit_message>
solved 163, 167, 169
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\study\python\DS-450-python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C303A9A2-C101-4775-A7AE-D44F1E567100}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2856FEE8-F26A-4816-A9A5-133C1555CEFB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="8100" yWindow="2775" windowWidth="28800" windowHeight="11385" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1854,8 +1854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A149" workbookViewId="0">
-      <selection activeCell="C163" sqref="C163"/>
+    <sheetView tabSelected="1" topLeftCell="A158" workbookViewId="0">
+      <selection activeCell="B170" sqref="B170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3565,7 +3565,7 @@
         <v>159</v>
       </c>
       <c r="C163" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="164" spans="1:3" ht="21">
@@ -3609,7 +3609,7 @@
         <v>163</v>
       </c>
       <c r="C167" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="168" spans="1:3" ht="21">
@@ -3631,7 +3631,7 @@
         <v>165</v>
       </c>
       <c r="C169" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="170" spans="1:3" ht="21">

</xml_diff>

<commit_message>
solved Linked List Problems 171, 172, 173
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\study\python\DS-450-python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\study\python coding\DS-450-python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2856FEE8-F26A-4816-A9A5-133C1555CEFB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7D358F4-69E1-4612-BF16-5C945B315E66}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8100" yWindow="2775" windowWidth="28800" windowHeight="11385" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1854,18 +1854,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A158" workbookViewId="0">
-      <selection activeCell="B170" sqref="B170"/>
+    <sheetView tabSelected="1" topLeftCell="A176" workbookViewId="0">
+      <selection activeCell="B354" sqref="B354"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="28.5" customWidth="1"/>
     <col min="2" max="2" width="123" customWidth="1"/>
     <col min="3" max="3" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="26.25">
+    <row r="1" spans="1:3" ht="24.6">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3326,7 +3326,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="142" spans="1:3" ht="19.5">
+    <row r="142" spans="1:3" ht="19.8">
       <c r="A142" s="8" t="s">
         <v>134</v>
       </c>
@@ -3499,7 +3499,7 @@
         <v>153</v>
       </c>
       <c r="C157" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="158" spans="1:3" ht="21">
@@ -3532,7 +3532,7 @@
         <v>156</v>
       </c>
       <c r="C160" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="161" spans="1:3" ht="21">
@@ -3576,7 +3576,7 @@
         <v>160</v>
       </c>
       <c r="C164" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="165" spans="1:3" ht="21">
@@ -3587,7 +3587,7 @@
         <v>161</v>
       </c>
       <c r="C165" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="166" spans="1:3" ht="21">
@@ -3653,7 +3653,7 @@
         <v>167</v>
       </c>
       <c r="C171" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="172" spans="1:3" ht="21">
@@ -3664,7 +3664,7 @@
         <v>168</v>
       </c>
       <c r="C172" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="173" spans="1:3" ht="21">
@@ -3675,7 +3675,7 @@
         <v>169</v>
       </c>
       <c r="C173" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="174" spans="1:3" ht="21">

</xml_diff>

<commit_message>
solved some linked list problems 139, 151, 168, 170
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\study\python coding\DS-450-python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7D358F4-69E1-4612-BF16-5C945B315E66}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52C084D3-C1F1-45C2-BB45-1F89E88F7336}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1854,8 +1854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A176" workbookViewId="0">
-      <selection activeCell="B354" sqref="B354"/>
+    <sheetView tabSelected="1" topLeftCell="A135" workbookViewId="0">
+      <selection activeCell="C139" sqref="C139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
@@ -3301,7 +3301,7 @@
         <v>135</v>
       </c>
       <c r="C139" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="140" spans="1:3" ht="21">
@@ -3433,7 +3433,7 @@
         <v>147</v>
       </c>
       <c r="C151" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="152" spans="1:3" ht="21">
@@ -3642,7 +3642,7 @@
         <v>166</v>
       </c>
       <c r="C170" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="171" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Solved Array Problems 7, 8, 9
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\study\python coding\DS-450-python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\study\python\DS-450-python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7D358F4-69E1-4612-BF16-5C945B315E66}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63707F87-22DD-4A90-ACFA-4015842BEEE1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="4710" yWindow="2565" windowWidth="28800" windowHeight="11385" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1351" uniqueCount="466">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1854,18 +1854,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A176" workbookViewId="0">
-      <selection activeCell="B354" sqref="B354"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="28.5" customWidth="1"/>
     <col min="2" max="2" width="123" customWidth="1"/>
     <col min="3" max="3" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="24.6">
+    <row r="1" spans="1:3" ht="26.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1887,9 +1887,7 @@
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="C5" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="C5" s="4"/>
     </row>
     <row r="6" spans="1:3" ht="21">
       <c r="A6" s="5" t="s">
@@ -1899,7 +1897,7 @@
         <v>6</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="21">
@@ -1910,7 +1908,7 @@
         <v>7</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="21">
@@ -1921,7 +1919,7 @@
         <v>8</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="21">
@@ -1932,7 +1930,7 @@
         <v>9</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="21">
@@ -3326,7 +3324,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="142" spans="1:3" ht="19.8">
+    <row r="142" spans="1:3" ht="19.5">
       <c r="A142" s="8" t="s">
         <v>134</v>
       </c>

</xml_diff>

<commit_message>
Solved Some array problems 10, 11, 12, 13
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\study\python\DS-450-python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63707F87-22DD-4A90-ACFA-4015842BEEE1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58AFC21B-C4A3-450B-9CFE-7C013E805F3D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4710" yWindow="2565" windowWidth="28800" windowHeight="11385" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="450" yWindow="1800" windowWidth="28800" windowHeight="11385" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1854,8 +1854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1941,7 +1941,7 @@
         <v>10</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="21">
@@ -1952,7 +1952,7 @@
         <v>11</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="21">
@@ -1963,7 +1963,7 @@
         <v>12</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="21">
@@ -1974,7 +1974,7 @@
         <v>13</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="21">

</xml_diff>

<commit_message>
solved some stack questions
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\study\python\DS-450-python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58AFC21B-C4A3-450B-9CFE-7C013E805F3D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{993FBEAE-0164-494B-B3FA-9EAB15A2755E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="450" yWindow="1800" windowWidth="28800" windowHeight="11385" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1854,8 +1854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A302" workbookViewId="0">
+      <selection activeCell="B324" sqref="B324"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -4954,7 +4954,7 @@
         <v>286</v>
       </c>
       <c r="C296" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="297" spans="1:3" ht="21">
@@ -4965,7 +4965,7 @@
         <v>287</v>
       </c>
       <c r="C297" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="298" spans="1:3" ht="21">
@@ -4976,7 +4976,7 @@
         <v>288</v>
       </c>
       <c r="C298" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="299" spans="1:3" ht="21">
@@ -4987,7 +4987,7 @@
         <v>289</v>
       </c>
       <c r="C299" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="300" spans="1:3" ht="21">
@@ -4998,7 +4998,7 @@
         <v>290</v>
       </c>
       <c r="C300" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="301" spans="1:3" ht="21">
@@ -5009,7 +5009,7 @@
         <v>291</v>
       </c>
       <c r="C301" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="302" spans="1:3" ht="21">
@@ -5020,7 +5020,7 @@
         <v>292</v>
       </c>
       <c r="C302" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="303" spans="1:3" ht="21">
@@ -5031,7 +5031,7 @@
         <v>293</v>
       </c>
       <c r="C303" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="304" spans="1:3" ht="21">
@@ -5042,7 +5042,7 @@
         <v>294</v>
       </c>
       <c r="C304" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="305" spans="1:3" ht="21">
@@ -5053,7 +5053,7 @@
         <v>295</v>
       </c>
       <c r="C305" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="306" spans="1:3" ht="21">
@@ -5064,7 +5064,7 @@
         <v>296</v>
       </c>
       <c r="C306" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="307" spans="1:3" ht="21">
@@ -5075,7 +5075,7 @@
         <v>297</v>
       </c>
       <c r="C307" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="308" spans="1:3" ht="21">
@@ -5086,7 +5086,7 @@
         <v>298</v>
       </c>
       <c r="C308" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="309" spans="1:3" ht="21">
@@ -5097,7 +5097,7 @@
         <v>299</v>
       </c>
       <c r="C309" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="310" spans="1:3" ht="21">
@@ -5130,7 +5130,7 @@
         <v>302</v>
       </c>
       <c r="C312" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="313" spans="1:3" ht="21">
@@ -5163,7 +5163,7 @@
         <v>305</v>
       </c>
       <c r="C315" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="316" spans="1:3" ht="21">
@@ -5174,7 +5174,7 @@
         <v>306</v>
       </c>
       <c r="C316" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="317" spans="1:3" ht="21">
@@ -5361,7 +5361,7 @@
         <v>323</v>
       </c>
       <c r="C333" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="334" spans="1:3" ht="21">

</xml_diff>

<commit_message>
solved some more stack questions
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\study\python\DS-450-python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{993FBEAE-0164-494B-B3FA-9EAB15A2755E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69C671DB-F9D2-46EB-AFB7-B08FA08AAA25}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1854,8 +1854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A302" workbookViewId="0">
-      <selection activeCell="B324" sqref="B324"/>
+    <sheetView tabSelected="1" topLeftCell="A314" workbookViewId="0">
+      <selection activeCell="C318" sqref="C318"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -5108,7 +5108,7 @@
         <v>300</v>
       </c>
       <c r="C310" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="311" spans="1:3" ht="21">
@@ -5141,7 +5141,7 @@
         <v>303</v>
       </c>
       <c r="C313" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="314" spans="1:3" ht="21">
@@ -5152,7 +5152,7 @@
         <v>304</v>
       </c>
       <c r="C314" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="315" spans="1:3" ht="21">
@@ -5185,7 +5185,7 @@
         <v>307</v>
       </c>
       <c r="C317" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="318" spans="1:3" ht="21">
@@ -5196,7 +5196,7 @@
         <v>308</v>
       </c>
       <c r="C318" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="319" spans="1:3" ht="21">
@@ -5218,7 +5218,7 @@
         <v>310</v>
       </c>
       <c r="C320" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="321" spans="1:3" ht="21">

</xml_diff>

<commit_message>
added LRU and reverse queue
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\study\python\DS-450-python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69C671DB-F9D2-46EB-AFB7-B08FA08AAA25}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9952024-3EB8-4C45-82A4-A92A3520DD18}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="450" yWindow="1800" windowWidth="28800" windowHeight="11385" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1854,8 +1854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A314" workbookViewId="0">
-      <selection activeCell="C318" sqref="C318"/>
+    <sheetView tabSelected="1" topLeftCell="A290" workbookViewId="0">
+      <selection activeCell="C319" sqref="C319"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -5229,7 +5229,7 @@
         <v>311</v>
       </c>
       <c r="C321" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="322" spans="1:3" ht="21">
@@ -5240,7 +5240,7 @@
         <v>312</v>
       </c>
       <c r="C322" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="323" spans="1:3" ht="21">

</xml_diff>

<commit_message>
solved some more stack&queue questions
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\study\python\DS-450-python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9952024-3EB8-4C45-82A4-A92A3520DD18}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6AE0C78-4858-4D74-B808-1627DDBAACD6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="450" yWindow="1800" windowWidth="28800" windowHeight="11385" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1854,8 +1854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A290" workbookViewId="0">
-      <selection activeCell="C319" sqref="C319"/>
+    <sheetView tabSelected="1" topLeftCell="A316" workbookViewId="0">
+      <selection activeCell="B330" sqref="B330"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -5207,7 +5207,7 @@
         <v>309</v>
       </c>
       <c r="C319" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="320" spans="1:3" ht="21">
@@ -5251,7 +5251,7 @@
         <v>313</v>
       </c>
       <c r="C323" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="324" spans="1:3" ht="21">
@@ -5262,7 +5262,7 @@
         <v>314</v>
       </c>
       <c r="C324" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="325" spans="1:3" ht="21">
@@ -5273,7 +5273,7 @@
         <v>315</v>
       </c>
       <c r="C325" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="326" spans="1:3" ht="21">

</xml_diff>

<commit_message>
stack and sliding windows questions solved
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\study\python\DS-450-python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6AE0C78-4858-4D74-B808-1627DDBAACD6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DBEB53C-F9A6-46BF-9269-33E6023A41A5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1855,7 +1855,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A316" workbookViewId="0">
-      <selection activeCell="B330" sqref="B330"/>
+      <selection activeCell="C329" sqref="C329"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -5306,7 +5306,7 @@
         <v>318</v>
       </c>
       <c r="C328" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="329" spans="1:3" ht="21">
@@ -5317,7 +5317,7 @@
         <v>319</v>
       </c>
       <c r="C329" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="330" spans="1:3" ht="21">
@@ -5328,7 +5328,7 @@
         <v>320</v>
       </c>
       <c r="C330" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="331" spans="1:3" ht="21">

</xml_diff>

<commit_message>
solved some bit manupulation questions
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\study\python\DS-450-python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1871077-61DC-4AAC-8437-A291F4A3FE1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59FB84C6-AD5C-4B67-A52C-021620BCCE3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1855,7 +1855,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A268" workbookViewId="0">
-      <selection activeCell="B285" sqref="B285"/>
+      <selection activeCell="C285" sqref="C285"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -4770,7 +4770,7 @@
         <v>269</v>
       </c>
       <c r="C278" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="279" spans="1:3" ht="21">
@@ -4792,7 +4792,7 @@
         <v>271</v>
       </c>
       <c r="C280" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="281" spans="1:3" ht="21">
@@ -4858,7 +4858,7 @@
         <v>277</v>
       </c>
       <c r="C286" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="287" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Added more on bit manipulations
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\study\python\DS-450-python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59FB84C6-AD5C-4B67-A52C-021620BCCE3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEA2A0DB-F1ED-4938-893B-322B779912EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="5445" yWindow="45" windowWidth="28800" windowHeight="11385" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1854,8 +1854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A268" workbookViewId="0">
-      <selection activeCell="C285" sqref="C285"/>
+    <sheetView tabSelected="1" topLeftCell="A469" workbookViewId="0">
+      <selection activeCell="C473" sqref="C473"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -6821,7 +6821,7 @@
         <v>454</v>
       </c>
       <c r="C472" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="473" spans="1:3" ht="21">
@@ -6832,7 +6832,7 @@
         <v>455</v>
       </c>
       <c r="C473" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="474" spans="1:3" ht="21">
@@ -6843,7 +6843,7 @@
         <v>456</v>
       </c>
       <c r="C474" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="475" spans="1:3" ht="21">
@@ -6854,7 +6854,7 @@
         <v>457</v>
       </c>
       <c r="C475" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="476" spans="1:3" ht="21">
@@ -6865,7 +6865,7 @@
         <v>458</v>
       </c>
       <c r="C476" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="477" spans="1:3" ht="21">
@@ -6898,7 +6898,7 @@
         <v>461</v>
       </c>
       <c r="C479" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="480" spans="1:3" ht="21">

</xml_diff>

<commit_message>
added bit manupulation and string finding algos
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\study\python\DS-450-python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEA2A0DB-F1ED-4938-893B-322B779912EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{897C5FF1-78F1-4D10-BF88-F961137151BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5445" yWindow="45" windowWidth="28800" windowHeight="11385" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="5445" yWindow="45" windowWidth="28710" windowHeight="11385" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1854,8 +1854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A469" workbookViewId="0">
-      <selection activeCell="C473" sqref="C473"/>
+    <sheetView tabSelected="1" topLeftCell="A467" workbookViewId="0">
+      <selection activeCell="B478" sqref="B478"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -6876,7 +6876,7 @@
         <v>459</v>
       </c>
       <c r="C477" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="478" spans="1:3" ht="21">

</xml_diff>

<commit_message>
added a lot of solutions
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\study\python\DS-450-python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{897C5FF1-78F1-4D10-BF88-F961137151BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6698E3DA-86E3-41DE-97A5-34DFBF159D59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5445" yWindow="45" windowWidth="28710" windowHeight="11385" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1854,8 +1854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A467" workbookViewId="0">
-      <selection activeCell="B478" sqref="B478"/>
+    <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
+      <selection activeCell="B180" sqref="B180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2608,7 +2608,7 @@
         <v>71</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="21">
@@ -2619,7 +2619,7 @@
         <v>72</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="21">
@@ -3699,7 +3699,7 @@
         <v>172</v>
       </c>
       <c r="C177" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="178" spans="1:3" ht="21">
@@ -3710,7 +3710,7 @@
         <v>173</v>
       </c>
       <c r="C178" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="179" spans="1:3" ht="21">
@@ -3721,7 +3721,7 @@
         <v>174</v>
       </c>
       <c r="C179" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="180" spans="1:3" ht="21">
@@ -6909,7 +6909,7 @@
         <v>462</v>
       </c>
       <c r="C480" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="481" spans="1:3" ht="21">
@@ -6920,7 +6920,7 @@
         <v>463</v>
       </c>
       <c r="C481" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added a lot of solutions, on two pointers, binary tree, bit manupulation
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\study\python\DS-450-python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6698E3DA-86E3-41DE-97A5-34DFBF159D59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D314A830-3615-4860-94D1-BE75807143EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="5445" yWindow="45" windowWidth="28710" windowHeight="11385" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1854,8 +1854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
-      <selection activeCell="B180" sqref="B180"/>
+    <sheetView tabSelected="1" topLeftCell="A176" workbookViewId="0">
+      <selection activeCell="B184" sqref="B184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3732,7 +3732,7 @@
         <v>175</v>
       </c>
       <c r="C180" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="181" spans="1:3" ht="21">
@@ -3743,7 +3743,7 @@
         <v>176</v>
       </c>
       <c r="C181" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="182" spans="1:3" ht="21">
@@ -3754,7 +3754,7 @@
         <v>177</v>
       </c>
       <c r="C182" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="183" spans="1:3" ht="21">
@@ -3765,7 +3765,7 @@
         <v>178</v>
       </c>
       <c r="C183" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="184" spans="1:3" ht="21">
@@ -3776,7 +3776,7 @@
         <v>179</v>
       </c>
       <c r="C184" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="185" spans="1:3" ht="21">
@@ -3787,7 +3787,7 @@
         <v>180</v>
       </c>
       <c r="C185" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="186" spans="1:3" ht="21">
@@ -3798,7 +3798,7 @@
         <v>181</v>
       </c>
       <c r="C186" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="187" spans="1:3" ht="21">

</xml_diff>

<commit_message>
added binary tree and two pointers solutions
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\study\python\DS-450-python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D314A830-3615-4860-94D1-BE75807143EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5C12ECE-24BD-476E-BC92-803F6A6F2978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5445" yWindow="45" windowWidth="28710" windowHeight="11385" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1351" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1351" uniqueCount="467">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1423,6 +1423,9 @@
   </si>
   <si>
     <t>yes</t>
+  </si>
+  <si>
+    <t>res</t>
   </si>
 </sst>
 </file>
@@ -1854,8 +1857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A176" workbookViewId="0">
-      <selection activeCell="B184" sqref="B184"/>
+    <sheetView tabSelected="1" topLeftCell="A182" workbookViewId="0">
+      <selection activeCell="B193" sqref="B193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3842,7 +3845,7 @@
         <v>185</v>
       </c>
       <c r="C190" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="191" spans="1:3" ht="21">
@@ -3853,7 +3856,7 @@
         <v>186</v>
       </c>
       <c r="C191" s="4" t="s">
-        <v>4</v>
+        <v>466</v>
       </c>
     </row>
     <row r="192" spans="1:3" ht="21">
@@ -3864,7 +3867,7 @@
         <v>187</v>
       </c>
       <c r="C192" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="193" spans="1:3" ht="21">

</xml_diff>

<commit_message>
after a long time commit
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\study\python\DS-450-python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5C12ECE-24BD-476E-BC92-803F6A6F2978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E72FFD0F-77E2-4DAA-9B09-717F4DEE4354}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5445" yWindow="45" windowWidth="28710" windowHeight="11385" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1857,13 +1857,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A182" workbookViewId="0">
-      <selection activeCell="B193" sqref="B193"/>
+    <sheetView tabSelected="1" topLeftCell="A403" workbookViewId="0">
+      <selection activeCell="C419" sqref="C419"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="28.5" customWidth="1"/>
+    <col min="1" max="1" width="25.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="123" customWidth="1"/>
     <col min="3" max="3" width="27.5" customWidth="1"/>
   </cols>
@@ -3434,7 +3434,7 @@
         <v>147</v>
       </c>
       <c r="C151" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="152" spans="1:3" ht="21">
@@ -6155,7 +6155,7 @@
         <v>394</v>
       </c>
       <c r="C410" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="411" spans="1:3" ht="21">
@@ -6166,7 +6166,7 @@
         <v>395</v>
       </c>
       <c r="C411" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="412" spans="1:3" ht="21">
@@ -6177,7 +6177,7 @@
         <v>396</v>
       </c>
       <c r="C412" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="413" spans="1:3" ht="21">
@@ -6188,7 +6188,7 @@
         <v>397</v>
       </c>
       <c r="C413" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="414" spans="1:3" ht="21">
@@ -6199,7 +6199,7 @@
         <v>398</v>
       </c>
       <c r="C414" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="415" spans="1:3" ht="21">
@@ -6210,7 +6210,7 @@
         <v>399</v>
       </c>
       <c r="C415" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="416" spans="1:3" ht="21">
@@ -6232,7 +6232,7 @@
         <v>273</v>
       </c>
       <c r="C417" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="418" spans="1:3" ht="21">
@@ -6254,7 +6254,7 @@
         <v>402</v>
       </c>
       <c r="C419" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="420" spans="1:3" ht="21">

</xml_diff>